<commit_message>
Manejo de Atributos Perfiles
</commit_message>
<xml_diff>
--- a/Libro2_actualizado.xlsx
+++ b/Libro2_actualizado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeronimo Vargas\OneDrive\Documentos\10 SEMESTRE\TESIS IIND-ISIS\REPOSITORIO\ciclorutas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8340A4FA-D2C3-44C6-BFC2-604F243823BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687318FA-CF61-42EF-82D4-3660431615BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NODOS" sheetId="1" r:id="rId1"/>
@@ -637,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220A9FBB-2E7B-4C7C-9740-D717B4AA7E5A}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA9026-958D-474F-AC15-4AB8D88D8110}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>